<commit_message>
End of the lecture about Reservoirs
</commit_message>
<xml_diff>
--- a/Vagasfinal.xlsx
+++ b/Vagasfinal.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DVH0\rearrange\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BF02E06-F7CC-4B96-9326-D249AE4A89E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BE3A7A0-25BD-4209-859B-5C7D4FB55011}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{FBD3203A-12B5-4F12-A2EC-6D55F28A17C7}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="72">
   <si>
     <t>Competência técnica</t>
   </si>
@@ -246,6 +246,12 @@
   </si>
   <si>
     <t>Caputra e armazenamento geológico de Carbona CC(U)S</t>
+  </si>
+  <si>
+    <t>Proximidade com Geociências</t>
+  </si>
+  <si>
+    <t>Pós-graduação</t>
   </si>
 </sst>
 </file>
@@ -298,7 +304,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -329,8 +335,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="12">
+  <borders count="20">
     <border>
       <left/>
       <right/>
@@ -497,15 +515,124 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -515,6 +642,7 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
@@ -528,14 +656,30 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -904,10 +1048,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D97DA5E7-41A8-47E6-88D5-2343F8D77AE1}">
-  <dimension ref="A1:F63"/>
+  <dimension ref="A1:E65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="B64" sqref="B64"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C60" sqref="C60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -915,7 +1059,8 @@
     <col min="1" max="1" width="23.7265625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="48.36328125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="60.08984375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="43.90625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="69.36328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="48.36328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
@@ -969,30 +1114,30 @@
     </row>
     <row r="15" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="16" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A16" s="8" t="s">
+      <c r="A16" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B16" s="9" t="s">
+      <c r="B16" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C16" s="10" t="s">
+      <c r="C16" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D16" s="7"/>
-      <c r="E16" s="6"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="5"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A17" s="11" t="s">
+      <c r="A17" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="B17" s="4" t="s">
+      <c r="B17" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C17" s="12" t="s">
+      <c r="C17" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="D17" s="5"/>
-      <c r="E17" s="6"/>
+      <c r="D17" s="4"/>
+      <c r="E17" s="5"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" s="17" t="s">
@@ -1004,19 +1149,19 @@
       <c r="C18" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="E18" s="6"/>
+      <c r="E18" s="5"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="B19" s="4" t="s">
+      <c r="B19" s="3" t="s">
         <v>10</v>
       </c>
       <c r="C19" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="E19" s="6"/>
+      <c r="E19" s="5"/>
     </row>
     <row r="20" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A20" s="13" t="s">
@@ -1028,20 +1173,20 @@
       <c r="C20" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="E20" s="6"/>
+      <c r="E20" s="5"/>
     </row>
     <row r="21" spans="1:5" ht="32.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="6" t="s">
+      <c r="A21" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B21" s="5" t="s">
+      <c r="B21" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C21" s="5" t="s">
+      <c r="C21" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="D21" s="5"/>
-      <c r="E21" s="6"/>
+      <c r="D21" s="4"/>
+      <c r="E21" s="5"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B22" t="s">
@@ -1050,7 +1195,7 @@
       <c r="C22" t="s">
         <v>17</v>
       </c>
-      <c r="D22" s="5"/>
+      <c r="D22" s="4"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B23" t="s">
@@ -1066,217 +1211,270 @@
         <v>22</v>
       </c>
     </row>
+    <row r="26" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="27" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B27" s="24" t="s">
+      <c r="B27" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="C27" s="24" t="s">
+      <c r="C27" s="31" t="s">
         <v>26</v>
       </c>
+      <c r="D27" s="35" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B28" t="s">
+      <c r="B28" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="C28" t="s">
+      <c r="C28" s="32" t="s">
         <v>27</v>
       </c>
+      <c r="D28" s="36" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="C29" s="25" t="s">
+      <c r="B29" s="10"/>
+      <c r="C29" s="33" t="s">
         <v>28</v>
       </c>
+      <c r="D29" s="36" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="C30" s="25" t="s">
+      <c r="B30" s="10"/>
+      <c r="C30" s="33" t="s">
         <v>29</v>
       </c>
+      <c r="D30" s="36" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A31" t="s">
+      <c r="A31" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B31" s="38" t="s">
         <v>31</v>
       </c>
-      <c r="C31" t="s">
+      <c r="C31" s="32" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A32" t="s">
+      <c r="D31" s="36" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A32" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B32" s="39" t="s">
         <v>34</v>
       </c>
-      <c r="C32" s="25" t="s">
+      <c r="C32" s="34" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="D32" s="36" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D33" s="37" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="B36" s="24" t="s">
+    <row r="35" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B36" s="25" t="s">
         <v>37</v>
       </c>
-      <c r="C36" s="24" t="s">
+      <c r="C36" s="27" t="s">
         <v>40</v>
       </c>
-      <c r="D36" s="24" t="s">
+      <c r="D36" s="26" t="s">
         <v>61</v>
       </c>
-      <c r="E36" s="24"/>
-      <c r="F36" s="24"/>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A37" s="27" t="s">
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A37" s="40" t="s">
         <v>44</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B37" s="41" t="s">
         <v>38</v>
       </c>
-      <c r="C37" t="s">
+      <c r="C37" s="42" t="s">
         <v>41</v>
       </c>
-      <c r="D37" t="s">
+      <c r="D37" s="43" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A38" s="27"/>
-      <c r="B38" t="s">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A38" s="40"/>
+      <c r="B38" s="41" t="s">
         <v>39</v>
       </c>
-      <c r="C38" t="s">
+      <c r="C38" s="42" t="s">
         <v>42</v>
       </c>
-      <c r="D38" t="s">
+      <c r="D38" s="43" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A39" s="26"/>
-      <c r="B39" s="3" t="s">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A39" s="24"/>
+      <c r="B39" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="D39" t="s">
+      <c r="C39" s="3"/>
+      <c r="D39" s="11" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A40" s="26"/>
-      <c r="B40" t="s">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A40" s="24"/>
+      <c r="B40" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="D40" t="s">
+      <c r="C40" s="3"/>
+      <c r="D40" s="11" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A41" s="26"/>
-      <c r="B41" t="s">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A41" s="24"/>
+      <c r="B41" s="10" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A42" s="26"/>
-      <c r="B42" t="s">
+      <c r="C41" s="3"/>
+      <c r="D41" s="11"/>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A42" s="24"/>
+      <c r="B42" s="10" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="B43" t="s">
+      <c r="C42" s="3"/>
+      <c r="D42" s="11"/>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B43" s="10" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="B44" t="s">
+      <c r="C43" s="3"/>
+      <c r="D43" s="11"/>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B44" s="10" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="B45" t="s">
+      <c r="C44" s="3"/>
+      <c r="D44" s="11"/>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B45" s="10" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="B46" t="s">
+      <c r="C45" s="3"/>
+      <c r="D45" s="11"/>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B46" s="10" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="B47" t="s">
+      <c r="C46" s="3"/>
+      <c r="D46" s="11"/>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B47" s="10" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="B48" s="25" t="s">
+      <c r="C47" s="3"/>
+      <c r="D47" s="11"/>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B48" s="28" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="49" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B49" s="3" t="s">
+      <c r="C48" s="3"/>
+      <c r="D48" s="11"/>
+    </row>
+    <row r="49" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B49" s="12" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="50" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B50" s="25" t="s">
+      <c r="C49" s="3"/>
+      <c r="D49" s="11"/>
+    </row>
+    <row r="50" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B50" s="28" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="51" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B51" s="25" t="s">
+      <c r="C50" s="3"/>
+      <c r="D50" s="11"/>
+    </row>
+    <row r="51" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B51" s="28" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="52" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B52" s="25" t="s">
+      <c r="C51" s="3"/>
+      <c r="D51" s="11"/>
+    </row>
+    <row r="52" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B52" s="28" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="53" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B53" s="25" t="s">
+      <c r="C52" s="3"/>
+      <c r="D52" s="11"/>
+    </row>
+    <row r="53" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B53" s="28" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="54" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B54" s="25" t="s">
+      <c r="C53" s="3"/>
+      <c r="D53" s="11"/>
+    </row>
+    <row r="54" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B54" s="28" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="55" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B55" s="25" t="s">
+      <c r="C54" s="3"/>
+      <c r="D54" s="11"/>
+    </row>
+    <row r="55" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B55" s="29" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="59" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B59" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="60" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B60" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="61" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B61" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="62" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B62" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="63" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B63" t="s">
-        <v>69</v>
-      </c>
+      <c r="C55" s="14"/>
+      <c r="D55" s="30"/>
+    </row>
+    <row r="59" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B59" s="5"/>
+    </row>
+    <row r="60" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B60" s="5"/>
+    </row>
+    <row r="61" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B61" s="5"/>
+    </row>
+    <row r="62" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B62" s="5"/>
+    </row>
+    <row r="63" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B63" s="5"/>
+    </row>
+    <row r="64" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B64" s="5"/>
+    </row>
+    <row r="65" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B65" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>